<commit_message>
Fix #7675 cortex: blank materials_input.xlsx
</commit_message>
<xml_diff>
--- a/sirepo/package_data/template/cortex/lib/materials_input.xlsx
+++ b/sirepo/package_data/template/cortex/lib/materials_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anovak/projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anovak/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772A4A49-02BB-AA40-BE1C-86A52FCF9B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A38FE53-B6DD-A242-B46C-F9063E38CB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata and Settings" sheetId="4" r:id="rId1"/>
@@ -38,14 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Eurofer 97</t>
-  </si>
-  <si>
     <t>Density</t>
   </si>
   <si>
@@ -58,69 +55,6 @@
     <t>Element or Nuclide</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Cr</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>Mn</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>Ta</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>Fe</t>
-  </si>
-  <si>
-    <t>balance</t>
-  </si>
-  <si>
-    <t>Nb</t>
-  </si>
-  <si>
-    <t>Mo</t>
-  </si>
-  <si>
-    <t>Ni</t>
-  </si>
-  <si>
-    <t>Cu</t>
-  </si>
-  <si>
-    <t>Al</t>
-  </si>
-  <si>
-    <t>Ti</t>
-  </si>
-  <si>
-    <t>Si</t>
-  </si>
-  <si>
-    <t>Co</t>
-  </si>
-  <si>
     <t>Neutron Source</t>
   </si>
   <si>
@@ -229,9 +163,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>structural</t>
-  </si>
-  <si>
     <t>DEMO</t>
   </si>
   <si>
@@ -241,21 +172,6 @@
     <t>T1</t>
   </si>
   <si>
-    <t>10.1016/j.fusengdes.2018.06.027</t>
-  </si>
-  <si>
-    <t>As</t>
-  </si>
-  <si>
-    <t>Sn</t>
-  </si>
-  <si>
-    <t>Sb</t>
-  </si>
-  <si>
-    <t>Zr</t>
-  </si>
-  <si>
     <t>Density is available as function of temperature; value is given at 500 C</t>
   </si>
   <si>
@@ -274,9 +190,6 @@
     <t>Instructions</t>
   </si>
   <si>
-    <t>T5.1</t>
-  </si>
-  <si>
     <t>DOI (without https://doi.org) to cite where this information comes from; if no DOI, enter URL to source</t>
   </si>
   <si>
@@ -349,15 +262,6 @@
     <t>Units used for this property in SI (kg, Pa, m, s)</t>
   </si>
   <si>
-    <t>kg/m3</t>
-  </si>
-  <si>
-    <t>W/m/K</t>
-  </si>
-  <si>
-    <t>Add addditional independent variables as columns as needed.</t>
-  </si>
-  <si>
     <t>yield strength</t>
   </si>
   <si>
@@ -421,10 +325,7 @@
     <t>(kg, Pa, m, s)</t>
   </si>
   <si>
-    <t>EXP</t>
-  </si>
-  <si>
-    <t>T20.1</t>
+    <t>Add additional independent variables as columns as needed.</t>
   </si>
 </sst>
 </file>
@@ -432,8 +333,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -712,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -727,20 +628,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -752,7 +649,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -761,12 +658,8 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -780,40 +673,28 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -827,6 +708,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1052,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83076E2C-424E-AC41-A2A5-1E7D770F2FF6}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1062,303 +958,299 @@
     <col min="2" max="4" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="1" spans="1:14" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>94</v>
+      <c r="A2" s="27" t="s">
+        <v>65</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
+      <c r="D2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>44</v>
+      <c r="B3" s="51"/>
+      <c r="C3" s="28" t="s">
+        <v>22</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
+        <v>55</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>43</v>
+      <c r="A4" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="51"/>
+      <c r="C4" s="28" t="s">
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
+        <v>56</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
-        <v>95</v>
+      <c r="A5" s="36" t="s">
+        <v>66</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="31" t="s">
-        <v>44</v>
+      <c r="C5" s="28" t="s">
+        <v>22</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
+        <v>67</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
-        <v>110</v>
+      <c r="A6" s="36" t="s">
+        <v>78</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="31" t="s">
-        <v>98</v>
+      <c r="C6" s="28" t="s">
+        <v>69</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
+        <v>79</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
-        <v>97</v>
+      <c r="A7" s="36" t="s">
+        <v>68</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="31" t="s">
-        <v>98</v>
+      <c r="C7" s="28" t="s">
+        <v>69</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-    </row>
-    <row r="8" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="38"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="61"/>
-      <c r="N8" s="61"/>
+        <v>70</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+    </row>
+    <row r="8" spans="1:14" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="30"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="34"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="52"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="12">
+        <v>35</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+    </row>
+    <row r="13" spans="1:14" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="32"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C14" s="28"/>
+    </row>
+    <row r="15" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="53"/>
+      <c r="C15" s="28"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="28"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="31"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="13">
+      <c r="D18" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-    </row>
-    <row r="13" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="36"/>
-    </row>
-    <row r="14" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="31"/>
-    </row>
-    <row r="15" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="54"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="31"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="31"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="62" t="s">
-        <v>122</v>
-      </c>
-      <c r="B24" s="62"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="63" t="s">
-        <v>123</v>
-      </c>
-      <c r="B25" s="64"/>
+      <c r="B25" s="56"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="65" t="s">
-        <v>124</v>
-      </c>
-      <c r="B26" s="66"/>
+      <c r="A26" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1375,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1008"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1386,570 +1278,430 @@
     <col min="8" max="26" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1" spans="1:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="50">
+        <v>7.625</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="25"/>
+    </row>
+    <row r="9" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
+      <c r="D9" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
+      <c r="D10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="59">
-        <v>7.625</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="27"/>
-    </row>
-    <row r="9" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="21" t="s">
-        <v>74</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:7" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
+      <c r="A15" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="60"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-    </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="44" t="s">
-        <v>37</v>
+      <c r="B17" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="40" t="s">
+        <v>15</v>
       </c>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="53" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="54">
-        <v>0.11</v>
-      </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="54">
-        <v>9</v>
-      </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="54">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="54">
-        <v>0.4</v>
-      </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="54"/>
-      <c r="C22" s="54">
-        <v>0.15</v>
-      </c>
-      <c r="D22" s="54">
-        <v>0.25</v>
-      </c>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
+      <c r="A22" s="46"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="54">
-        <v>0.12</v>
-      </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
       <c r="L23" s="3"/>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="54">
-        <v>0.03</v>
-      </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="55" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="54">
-        <v>0</v>
-      </c>
-      <c r="D25" s="54">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
       <c r="L25" s="4"/>
       <c r="O25" s="1"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="54">
-        <v>0</v>
-      </c>
-      <c r="D26" s="54">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
+      <c r="A26" s="46"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="55" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="54">
-        <v>0</v>
-      </c>
-      <c r="D27" s="54">
-        <v>2E-3</v>
-      </c>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
+      <c r="A27" s="46"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="55" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54">
-        <v>0</v>
-      </c>
-      <c r="D28" s="54">
-        <v>0.01</v>
-      </c>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
+      <c r="A28" s="46"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="54"/>
+      <c r="A29" s="46"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54">
-        <v>0</v>
-      </c>
-      <c r="D30" s="54">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
+      <c r="A30" s="46"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="54"/>
-      <c r="C31" s="54">
-        <v>0</v>
-      </c>
-      <c r="D31" s="54">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
+      <c r="A31" s="46"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="54"/>
-      <c r="C32" s="54">
-        <v>0</v>
-      </c>
-      <c r="D32" s="54">
-        <v>0.01</v>
-      </c>
-      <c r="E32" s="54"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54"/>
+      <c r="A32" s="46"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="54"/>
-      <c r="C33" s="54">
-        <v>0</v>
-      </c>
-      <c r="D33" s="54">
-        <v>0.01</v>
-      </c>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
+      <c r="A33" s="46"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54">
-        <v>0</v>
-      </c>
-      <c r="D34" s="54">
-        <v>0.01</v>
-      </c>
-      <c r="E34" s="54"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="54"/>
+      <c r="A34" s="46"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="54"/>
-      <c r="C35" s="54">
-        <v>0</v>
-      </c>
-      <c r="D35" s="54">
-        <v>0.02</v>
-      </c>
-      <c r="E35" s="54"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="54"/>
+      <c r="A35" s="46"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="54"/>
-      <c r="C36" s="54">
-        <v>0</v>
-      </c>
-      <c r="D36" s="54">
-        <v>0.05</v>
-      </c>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
+      <c r="A36" s="46"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="54"/>
-      <c r="C37" s="54">
-        <v>0</v>
-      </c>
-      <c r="D37" s="54">
-        <v>0.01</v>
-      </c>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="54"/>
+      <c r="A37" s="46"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="55" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" s="54"/>
-      <c r="C38" s="54">
-        <v>0</v>
-      </c>
-      <c r="D38" s="54">
-        <f>0.05/4</f>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="54"/>
+      <c r="A38" s="46"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39" s="54"/>
-      <c r="C39" s="54">
-        <v>0</v>
-      </c>
-      <c r="D39" s="54">
-        <f>0.05/4</f>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="E39" s="54"/>
-      <c r="F39" s="54"/>
-      <c r="G39" s="54"/>
+      <c r="A39" s="46"/>
+      <c r="B39" s="45"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="45"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="55" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="54"/>
-      <c r="C40" s="54">
-        <v>0</v>
-      </c>
-      <c r="D40" s="54">
-        <f>0.05/4</f>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="E40" s="54"/>
-      <c r="F40" s="54"/>
-      <c r="G40" s="54"/>
+      <c r="A40" s="46"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="45"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="55" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="54"/>
-      <c r="C41" s="54">
-        <v>0</v>
-      </c>
-      <c r="D41" s="54">
-        <f>0.05/4</f>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="E41" s="54"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="54"/>
-    </row>
-    <row r="42" spans="1:7" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="A41" s="46"/>
+      <c r="B41" s="45"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
+    </row>
+    <row r="42" spans="1:7" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2931,8 +2683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0AC633-2A57-854D-9B48-48EF2D26487D}">
   <dimension ref="A1:S132"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2945,105 +2697,95 @@
     <col min="6" max="6" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="1" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="31" t="s">
-        <v>125</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="S2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="S3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="S4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="S5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="S6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="S3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="S4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="S5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="S6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="S7" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3051,313 +2793,244 @@
       <c r="B8" s="11"/>
       <c r="E8" s="5"/>
       <c r="S8" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="F9" s="17"/>
+      <c r="A9" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="15"/>
       <c r="S9" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="52">
-        <v>7.7439999999999998</v>
-      </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="9">
-        <f>20+273.15</f>
-        <v>293.14999999999998</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0</v>
-      </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
       <c r="S10" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="52">
-        <v>7.75</v>
-      </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="9">
-        <f>50+273.15</f>
-        <v>323.14999999999998</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0</v>
-      </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
       <c r="S11" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="52">
-        <v>7.74</v>
-      </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="9">
-        <f>100+273.15</f>
-        <v>373.15</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0</v>
-      </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
       <c r="S12" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="52">
-        <v>7.7229999999999999</v>
-      </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="9">
-        <f>200+273.15</f>
-        <v>473.15</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0</v>
-      </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
       <c r="S13" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="52">
-        <v>7.6909999999999998</v>
-      </c>
-      <c r="B14" s="52"/>
-      <c r="C14" s="51">
-        <v>573.15</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0</v>
-      </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
       <c r="S14" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="52">
-        <v>7.657</v>
-      </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="51">
-        <v>673.15</v>
-      </c>
-      <c r="D15" s="9">
-        <v>0</v>
-      </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="52">
-        <v>7.625</v>
-      </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="51">
-        <v>773.15</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0</v>
-      </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="52">
-        <v>7.5919999999999996</v>
-      </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="51">
-        <v>873.15</v>
-      </c>
-      <c r="D17" s="9">
-        <v>0</v>
-      </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="52">
-        <v>7.5590000000000002</v>
-      </c>
-      <c r="B18" s="52"/>
-      <c r="C18" s="9">
-        <f>700+273.15</f>
-        <v>973.15</v>
-      </c>
-      <c r="D18" s="9">
-        <v>0</v>
-      </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="52"/>
-      <c r="B19" s="52"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="52"/>
-      <c r="B20" s="52"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="52"/>
-      <c r="B21" s="52"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="43"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="52"/>
-      <c r="B22" s="52"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="43"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="52"/>
-      <c r="B23" s="52"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="43"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="52"/>
-      <c r="B24" s="52"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="43"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="52"/>
-      <c r="B25" s="52"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="43"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-    </row>
-    <row r="26" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>125</v>
+      <c r="A27" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="28" t="s">
+        <v>93</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>126</v>
+      <c r="A28" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="28" t="s">
+        <v>94</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>74</v>
+      <c r="A29" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="28" t="s">
+        <v>46</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C30" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="C31" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="50" t="s">
-        <v>74</v>
-      </c>
       <c r="D32" s="5" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3366,460 +3039,407 @@
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="F34" s="17"/>
+      <c r="A34" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F34" s="15"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="52">
-        <v>28.08</v>
-      </c>
-      <c r="B35" s="52"/>
-      <c r="C35" s="9">
-        <f>20+273.15</f>
-        <v>293.14999999999998</v>
-      </c>
-      <c r="D35" s="9">
-        <v>0</v>
-      </c>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="52">
-        <v>28.86</v>
-      </c>
-      <c r="B36" s="52"/>
-      <c r="C36" s="9">
-        <f>50+273.15</f>
-        <v>323.14999999999998</v>
-      </c>
-      <c r="D36" s="9">
-        <v>0</v>
-      </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="52">
-        <v>29.78</v>
-      </c>
-      <c r="B37" s="52"/>
-      <c r="C37" s="9">
-        <f>100+273.15</f>
-        <v>373.15</v>
-      </c>
-      <c r="D37" s="9">
-        <v>0</v>
-      </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="52">
-        <v>30.38</v>
-      </c>
-      <c r="B38" s="52"/>
-      <c r="C38" s="9">
-        <f>200+273.15</f>
-        <v>473.15</v>
-      </c>
-      <c r="D38" s="9">
-        <v>0</v>
-      </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="52">
-        <v>30.01</v>
-      </c>
-      <c r="B39" s="52"/>
-      <c r="C39" s="51">
-        <v>573.15</v>
-      </c>
-      <c r="D39" s="9">
-        <v>0</v>
-      </c>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
+      <c r="A39" s="43"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="52">
-        <v>29.47</v>
-      </c>
-      <c r="B40" s="52"/>
-      <c r="C40" s="51">
-        <v>673.15</v>
-      </c>
-      <c r="D40" s="9">
-        <v>0</v>
-      </c>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
+      <c r="A40" s="43"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="52">
-        <v>29.58</v>
-      </c>
-      <c r="B41" s="52"/>
-      <c r="C41" s="51">
-        <v>773.15</v>
-      </c>
-      <c r="D41" s="9">
-        <v>0</v>
-      </c>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
+      <c r="A41" s="43"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="52">
-        <v>31.12</v>
-      </c>
-      <c r="B42" s="52"/>
-      <c r="C42" s="51">
-        <v>873.15</v>
-      </c>
-      <c r="D42" s="9">
-        <v>0</v>
-      </c>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="52"/>
-      <c r="B43" s="52"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="52"/>
-      <c r="B44" s="52"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="52"/>
-      <c r="B45" s="52"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="52"/>
-      <c r="B46" s="52"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="43"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="52"/>
-      <c r="B47" s="52"/>
+      <c r="A47" s="43"/>
+      <c r="B47" s="43"/>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="52"/>
-      <c r="B48" s="52"/>
+      <c r="A48" s="43"/>
+      <c r="B48" s="43"/>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="52"/>
-      <c r="B49" s="52"/>
+      <c r="A49" s="43"/>
+      <c r="B49" s="43"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="52"/>
-      <c r="B50" s="52"/>
+      <c r="A50" s="43"/>
+      <c r="B50" s="43"/>
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-    </row>
-    <row r="51" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="42" t="s">
-        <v>47</v>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+    </row>
+    <row r="51" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="38" t="s">
+        <v>25</v>
       </c>
       <c r="B52" s="9"/>
-      <c r="C52" s="31" t="s">
-        <v>125</v>
+      <c r="C52" s="28" t="s">
+        <v>93</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="E52"/>
     </row>
-    <row r="53" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="42" t="s">
-        <v>53</v>
+    <row r="53" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="38" t="s">
+        <v>31</v>
       </c>
       <c r="B53" s="9"/>
-      <c r="C53" s="31" t="s">
-        <v>126</v>
+      <c r="C53" s="28" t="s">
+        <v>94</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="E53"/>
     </row>
-    <row r="54" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="B54" s="20"/>
-      <c r="C54" s="31" t="s">
-        <v>74</v>
+    <row r="54" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B54" s="18"/>
+      <c r="C54" s="28" t="s">
+        <v>46</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="E54"/>
     </row>
-    <row r="55" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="40" t="s">
+    <row r="55" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" s="9"/>
+      <c r="C55" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E55"/>
+    </row>
+    <row r="56" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" s="9"/>
+      <c r="C56" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E56"/>
+    </row>
+    <row r="57" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B57" s="9"/>
+      <c r="C57" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E55"/>
-    </row>
-    <row r="56" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E56"/>
-    </row>
-    <row r="57" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="50" t="s">
-        <v>74</v>
-      </c>
       <c r="D57" s="5" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="E57"/>
-      <c r="F57" s="17"/>
-    </row>
-    <row r="58" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F57" s="15"/>
+    </row>
+    <row r="58" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="8"/>
-      <c r="B58" s="11"/>
       <c r="C58"/>
       <c r="D58"/>
       <c r="E58" s="5"/>
     </row>
-    <row r="59" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B59" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C59" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="D59" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="E59" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="52"/>
-      <c r="B60" s="52"/>
+    <row r="59" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D59" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="43"/>
+      <c r="B60" s="43"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
     </row>
-    <row r="61" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="52"/>
-      <c r="B61" s="52"/>
+    <row r="61" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="43"/>
+      <c r="B61" s="43"/>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
     </row>
-    <row r="62" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="52"/>
-      <c r="B62" s="52"/>
+    <row r="62" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="43"/>
+      <c r="B62" s="43"/>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
     </row>
-    <row r="63" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="52"/>
-      <c r="B63" s="52"/>
+    <row r="63" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="43"/>
+      <c r="B63" s="43"/>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
     </row>
-    <row r="64" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="52"/>
-      <c r="B64" s="52"/>
-      <c r="C64" s="51"/>
+    <row r="64" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="43"/>
+      <c r="B64" s="43"/>
+      <c r="C64" s="42"/>
       <c r="D64" s="9"/>
     </row>
-    <row r="65" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="52"/>
-      <c r="B65" s="52"/>
-      <c r="C65" s="51"/>
+    <row r="65" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="43"/>
+      <c r="B65" s="43"/>
+      <c r="C65" s="42"/>
       <c r="D65" s="9"/>
     </row>
-    <row r="66" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="52"/>
-      <c r="B66" s="52"/>
-      <c r="C66" s="51"/>
+    <row r="66" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="43"/>
+      <c r="B66" s="43"/>
+      <c r="C66" s="42"/>
       <c r="D66" s="9"/>
     </row>
-    <row r="67" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="52"/>
-      <c r="B67" s="52"/>
-      <c r="C67" s="51"/>
+    <row r="67" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="43"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="42"/>
       <c r="D67" s="9"/>
     </row>
-    <row r="68" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="52"/>
-      <c r="B68" s="52"/>
+    <row r="68" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="43"/>
+      <c r="B68" s="43"/>
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
     </row>
-    <row r="69" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="52"/>
-      <c r="B69" s="52"/>
+    <row r="69" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="43"/>
+      <c r="B69" s="43"/>
       <c r="C69" s="9"/>
       <c r="D69" s="9"/>
     </row>
-    <row r="70" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="52"/>
-      <c r="B70" s="52"/>
+    <row r="70" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="43"/>
+      <c r="B70" s="43"/>
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
     </row>
-    <row r="71" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="52"/>
-      <c r="B71" s="52"/>
+    <row r="71" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="43"/>
+      <c r="B71" s="43"/>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
     </row>
-    <row r="72" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="52"/>
-      <c r="B72" s="52"/>
+    <row r="72" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="43"/>
+      <c r="B72" s="43"/>
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
     </row>
-    <row r="73" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="52"/>
-      <c r="B73" s="52"/>
+    <row r="73" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="43"/>
+      <c r="B73" s="43"/>
       <c r="C73" s="9"/>
       <c r="D73" s="9"/>
     </row>
-    <row r="74" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="52"/>
-      <c r="B74" s="52"/>
+    <row r="74" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="43"/>
+      <c r="B74" s="43"/>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
     </row>
-    <row r="75" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="52"/>
-      <c r="B75" s="52"/>
+    <row r="75" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="43"/>
+      <c r="B75" s="43"/>
       <c r="C75" s="9"/>
       <c r="D75" s="9"/>
     </row>
-    <row r="76" spans="1:4" s="61" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="77" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="81" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="82" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="83" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="84" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="85" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="86" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="87" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="88" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="89" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="90" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="91" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="92" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="93" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="94" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="95" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="96" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="97" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="98" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="99" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="100" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="101" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="102" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="103" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="104" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="105" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="106" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="107" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="108" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="109" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="110" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="111" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="112" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="113" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="114" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="115" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="116" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="117" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="118" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="119" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="120" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="121" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="122" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="123" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="124" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="125" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="126" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="127" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="128" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="129" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="130" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="131" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="132" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="81" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="82" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="83" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="84" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="85" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="86" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="87" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="88" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="89" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="90" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="91" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="92" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="93" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="94" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="95" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="96" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="97" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="98" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="99" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="100" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="101" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="102" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="103" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="104" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="105" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="106" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="107" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="108" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="109" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="110" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="111" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="112" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="113" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="114" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="115" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="116" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="117" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="118" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="119" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="120" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="121" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="122" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="123" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="124" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="125" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="126" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="127" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="128" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="129" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="130" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="131" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="132" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B27 B52" xr:uid="{A0BF1BEF-0696-864B-BDBB-F02F002EAA73}">

</xml_diff>

<commit_message>
Fix #7675 cortex: blank materials_input.xlsx (#7676)
</commit_message>
<xml_diff>
--- a/sirepo/package_data/template/cortex/lib/materials_input.xlsx
+++ b/sirepo/package_data/template/cortex/lib/materials_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anovak/projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anovak/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772A4A49-02BB-AA40-BE1C-86A52FCF9B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A38FE53-B6DD-A242-B46C-F9063E38CB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata and Settings" sheetId="4" r:id="rId1"/>
@@ -38,14 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Eurofer 97</t>
-  </si>
-  <si>
     <t>Density</t>
   </si>
   <si>
@@ -58,69 +55,6 @@
     <t>Element or Nuclide</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Cr</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>Mn</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>Ta</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>Fe</t>
-  </si>
-  <si>
-    <t>balance</t>
-  </si>
-  <si>
-    <t>Nb</t>
-  </si>
-  <si>
-    <t>Mo</t>
-  </si>
-  <si>
-    <t>Ni</t>
-  </si>
-  <si>
-    <t>Cu</t>
-  </si>
-  <si>
-    <t>Al</t>
-  </si>
-  <si>
-    <t>Ti</t>
-  </si>
-  <si>
-    <t>Si</t>
-  </si>
-  <si>
-    <t>Co</t>
-  </si>
-  <si>
     <t>Neutron Source</t>
   </si>
   <si>
@@ -229,9 +163,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>structural</t>
-  </si>
-  <si>
     <t>DEMO</t>
   </si>
   <si>
@@ -241,21 +172,6 @@
     <t>T1</t>
   </si>
   <si>
-    <t>10.1016/j.fusengdes.2018.06.027</t>
-  </si>
-  <si>
-    <t>As</t>
-  </si>
-  <si>
-    <t>Sn</t>
-  </si>
-  <si>
-    <t>Sb</t>
-  </si>
-  <si>
-    <t>Zr</t>
-  </si>
-  <si>
     <t>Density is available as function of temperature; value is given at 500 C</t>
   </si>
   <si>
@@ -274,9 +190,6 @@
     <t>Instructions</t>
   </si>
   <si>
-    <t>T5.1</t>
-  </si>
-  <si>
     <t>DOI (without https://doi.org) to cite where this information comes from; if no DOI, enter URL to source</t>
   </si>
   <si>
@@ -349,15 +262,6 @@
     <t>Units used for this property in SI (kg, Pa, m, s)</t>
   </si>
   <si>
-    <t>kg/m3</t>
-  </si>
-  <si>
-    <t>W/m/K</t>
-  </si>
-  <si>
-    <t>Add addditional independent variables as columns as needed.</t>
-  </si>
-  <si>
     <t>yield strength</t>
   </si>
   <si>
@@ -421,10 +325,7 @@
     <t>(kg, Pa, m, s)</t>
   </si>
   <si>
-    <t>EXP</t>
-  </si>
-  <si>
-    <t>T20.1</t>
+    <t>Add additional independent variables as columns as needed.</t>
   </si>
 </sst>
 </file>
@@ -432,8 +333,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -712,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -727,20 +628,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -752,7 +649,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -761,12 +658,8 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -780,40 +673,28 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -827,6 +708,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1052,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83076E2C-424E-AC41-A2A5-1E7D770F2FF6}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1062,303 +958,299 @@
     <col min="2" max="4" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="1" spans="1:14" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>94</v>
+      <c r="A2" s="27" t="s">
+        <v>65</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
+      <c r="D2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>44</v>
+      <c r="B3" s="51"/>
+      <c r="C3" s="28" t="s">
+        <v>22</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
+        <v>55</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>43</v>
+      <c r="A4" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="51"/>
+      <c r="C4" s="28" t="s">
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
+        <v>56</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
-        <v>95</v>
+      <c r="A5" s="36" t="s">
+        <v>66</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="31" t="s">
-        <v>44</v>
+      <c r="C5" s="28" t="s">
+        <v>22</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
+        <v>67</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
-        <v>110</v>
+      <c r="A6" s="36" t="s">
+        <v>78</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="31" t="s">
-        <v>98</v>
+      <c r="C6" s="28" t="s">
+        <v>69</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
+        <v>79</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
-        <v>97</v>
+      <c r="A7" s="36" t="s">
+        <v>68</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="31" t="s">
-        <v>98</v>
+      <c r="C7" s="28" t="s">
+        <v>69</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-    </row>
-    <row r="8" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="38"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="61"/>
-      <c r="N8" s="61"/>
+        <v>70</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+    </row>
+    <row r="8" spans="1:14" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="30"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="34"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="52"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="12">
+        <v>35</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+    </row>
+    <row r="13" spans="1:14" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="32"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C14" s="28"/>
+    </row>
+    <row r="15" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="53"/>
+      <c r="C15" s="28"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="28"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="31"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="13">
+      <c r="D18" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-    </row>
-    <row r="13" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="36"/>
-    </row>
-    <row r="14" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="31"/>
-    </row>
-    <row r="15" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="54"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="31"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="31"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="62" t="s">
-        <v>122</v>
-      </c>
-      <c r="B24" s="62"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="63" t="s">
-        <v>123</v>
-      </c>
-      <c r="B25" s="64"/>
+      <c r="B25" s="56"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="65" t="s">
-        <v>124</v>
-      </c>
-      <c r="B26" s="66"/>
+      <c r="A26" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1375,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1008"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1386,570 +1278,430 @@
     <col min="8" max="26" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1" spans="1:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="50">
+        <v>7.625</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="25"/>
+    </row>
+    <row r="9" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
+      <c r="D9" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
+      <c r="D10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="59">
-        <v>7.625</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="27"/>
-    </row>
-    <row r="9" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="21" t="s">
-        <v>74</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:7" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
+      <c r="A15" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="60"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-    </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="44" t="s">
-        <v>37</v>
+      <c r="B17" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="40" t="s">
+        <v>15</v>
       </c>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="53" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="54">
-        <v>0.11</v>
-      </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="54">
-        <v>9</v>
-      </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="54">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="54">
-        <v>0.4</v>
-      </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="54"/>
-      <c r="C22" s="54">
-        <v>0.15</v>
-      </c>
-      <c r="D22" s="54">
-        <v>0.25</v>
-      </c>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
+      <c r="A22" s="46"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="54">
-        <v>0.12</v>
-      </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
       <c r="L23" s="3"/>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="54">
-        <v>0.03</v>
-      </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="55" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="54">
-        <v>0</v>
-      </c>
-      <c r="D25" s="54">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
       <c r="L25" s="4"/>
       <c r="O25" s="1"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="54">
-        <v>0</v>
-      </c>
-      <c r="D26" s="54">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
+      <c r="A26" s="46"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="55" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="54">
-        <v>0</v>
-      </c>
-      <c r="D27" s="54">
-        <v>2E-3</v>
-      </c>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
+      <c r="A27" s="46"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="55" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54">
-        <v>0</v>
-      </c>
-      <c r="D28" s="54">
-        <v>0.01</v>
-      </c>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
+      <c r="A28" s="46"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="54"/>
+      <c r="A29" s="46"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54">
-        <v>0</v>
-      </c>
-      <c r="D30" s="54">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
+      <c r="A30" s="46"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="54"/>
-      <c r="C31" s="54">
-        <v>0</v>
-      </c>
-      <c r="D31" s="54">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
+      <c r="A31" s="46"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="54"/>
-      <c r="C32" s="54">
-        <v>0</v>
-      </c>
-      <c r="D32" s="54">
-        <v>0.01</v>
-      </c>
-      <c r="E32" s="54"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54"/>
+      <c r="A32" s="46"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="54"/>
-      <c r="C33" s="54">
-        <v>0</v>
-      </c>
-      <c r="D33" s="54">
-        <v>0.01</v>
-      </c>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
+      <c r="A33" s="46"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54">
-        <v>0</v>
-      </c>
-      <c r="D34" s="54">
-        <v>0.01</v>
-      </c>
-      <c r="E34" s="54"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="54"/>
+      <c r="A34" s="46"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="54"/>
-      <c r="C35" s="54">
-        <v>0</v>
-      </c>
-      <c r="D35" s="54">
-        <v>0.02</v>
-      </c>
-      <c r="E35" s="54"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="54"/>
+      <c r="A35" s="46"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="54"/>
-      <c r="C36" s="54">
-        <v>0</v>
-      </c>
-      <c r="D36" s="54">
-        <v>0.05</v>
-      </c>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
+      <c r="A36" s="46"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="54"/>
-      <c r="C37" s="54">
-        <v>0</v>
-      </c>
-      <c r="D37" s="54">
-        <v>0.01</v>
-      </c>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="54"/>
+      <c r="A37" s="46"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="55" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" s="54"/>
-      <c r="C38" s="54">
-        <v>0</v>
-      </c>
-      <c r="D38" s="54">
-        <f>0.05/4</f>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="54"/>
+      <c r="A38" s="46"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39" s="54"/>
-      <c r="C39" s="54">
-        <v>0</v>
-      </c>
-      <c r="D39" s="54">
-        <f>0.05/4</f>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="E39" s="54"/>
-      <c r="F39" s="54"/>
-      <c r="G39" s="54"/>
+      <c r="A39" s="46"/>
+      <c r="B39" s="45"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="45"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="55" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="54"/>
-      <c r="C40" s="54">
-        <v>0</v>
-      </c>
-      <c r="D40" s="54">
-        <f>0.05/4</f>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="E40" s="54"/>
-      <c r="F40" s="54"/>
-      <c r="G40" s="54"/>
+      <c r="A40" s="46"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="45"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="55" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="54"/>
-      <c r="C41" s="54">
-        <v>0</v>
-      </c>
-      <c r="D41" s="54">
-        <f>0.05/4</f>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="E41" s="54"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="54"/>
-    </row>
-    <row r="42" spans="1:7" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="A41" s="46"/>
+      <c r="B41" s="45"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
+    </row>
+    <row r="42" spans="1:7" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2931,8 +2683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0AC633-2A57-854D-9B48-48EF2D26487D}">
   <dimension ref="A1:S132"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2945,105 +2697,95 @@
     <col min="6" max="6" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="1" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="31" t="s">
-        <v>125</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="S2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="S3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="S4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="S5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="S6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="S3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="S4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="S5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="S6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="S7" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3051,313 +2793,244 @@
       <c r="B8" s="11"/>
       <c r="E8" s="5"/>
       <c r="S8" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="F9" s="17"/>
+      <c r="A9" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="15"/>
       <c r="S9" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="52">
-        <v>7.7439999999999998</v>
-      </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="9">
-        <f>20+273.15</f>
-        <v>293.14999999999998</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0</v>
-      </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
       <c r="S10" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="52">
-        <v>7.75</v>
-      </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="9">
-        <f>50+273.15</f>
-        <v>323.14999999999998</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0</v>
-      </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
       <c r="S11" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="52">
-        <v>7.74</v>
-      </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="9">
-        <f>100+273.15</f>
-        <v>373.15</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0</v>
-      </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
       <c r="S12" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="52">
-        <v>7.7229999999999999</v>
-      </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="9">
-        <f>200+273.15</f>
-        <v>473.15</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0</v>
-      </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
       <c r="S13" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="52">
-        <v>7.6909999999999998</v>
-      </c>
-      <c r="B14" s="52"/>
-      <c r="C14" s="51">
-        <v>573.15</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0</v>
-      </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
       <c r="S14" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="52">
-        <v>7.657</v>
-      </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="51">
-        <v>673.15</v>
-      </c>
-      <c r="D15" s="9">
-        <v>0</v>
-      </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="52">
-        <v>7.625</v>
-      </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="51">
-        <v>773.15</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0</v>
-      </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="52">
-        <v>7.5919999999999996</v>
-      </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="51">
-        <v>873.15</v>
-      </c>
-      <c r="D17" s="9">
-        <v>0</v>
-      </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="52">
-        <v>7.5590000000000002</v>
-      </c>
-      <c r="B18" s="52"/>
-      <c r="C18" s="9">
-        <f>700+273.15</f>
-        <v>973.15</v>
-      </c>
-      <c r="D18" s="9">
-        <v>0</v>
-      </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="52"/>
-      <c r="B19" s="52"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="52"/>
-      <c r="B20" s="52"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="52"/>
-      <c r="B21" s="52"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="43"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="52"/>
-      <c r="B22" s="52"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="43"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="52"/>
-      <c r="B23" s="52"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="43"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="52"/>
-      <c r="B24" s="52"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="43"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="52"/>
-      <c r="B25" s="52"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="43"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-    </row>
-    <row r="26" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>125</v>
+      <c r="A27" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="28" t="s">
+        <v>93</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>126</v>
+      <c r="A28" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="28" t="s">
+        <v>94</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>74</v>
+      <c r="A29" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="28" t="s">
+        <v>46</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C30" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="C31" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="50" t="s">
-        <v>74</v>
-      </c>
       <c r="D32" s="5" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3366,460 +3039,407 @@
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="F34" s="17"/>
+      <c r="A34" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F34" s="15"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="52">
-        <v>28.08</v>
-      </c>
-      <c r="B35" s="52"/>
-      <c r="C35" s="9">
-        <f>20+273.15</f>
-        <v>293.14999999999998</v>
-      </c>
-      <c r="D35" s="9">
-        <v>0</v>
-      </c>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="52">
-        <v>28.86</v>
-      </c>
-      <c r="B36" s="52"/>
-      <c r="C36" s="9">
-        <f>50+273.15</f>
-        <v>323.14999999999998</v>
-      </c>
-      <c r="D36" s="9">
-        <v>0</v>
-      </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="52">
-        <v>29.78</v>
-      </c>
-      <c r="B37" s="52"/>
-      <c r="C37" s="9">
-        <f>100+273.15</f>
-        <v>373.15</v>
-      </c>
-      <c r="D37" s="9">
-        <v>0</v>
-      </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="52">
-        <v>30.38</v>
-      </c>
-      <c r="B38" s="52"/>
-      <c r="C38" s="9">
-        <f>200+273.15</f>
-        <v>473.15</v>
-      </c>
-      <c r="D38" s="9">
-        <v>0</v>
-      </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="52">
-        <v>30.01</v>
-      </c>
-      <c r="B39" s="52"/>
-      <c r="C39" s="51">
-        <v>573.15</v>
-      </c>
-      <c r="D39" s="9">
-        <v>0</v>
-      </c>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
+      <c r="A39" s="43"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="52">
-        <v>29.47</v>
-      </c>
-      <c r="B40" s="52"/>
-      <c r="C40" s="51">
-        <v>673.15</v>
-      </c>
-      <c r="D40" s="9">
-        <v>0</v>
-      </c>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
+      <c r="A40" s="43"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="52">
-        <v>29.58</v>
-      </c>
-      <c r="B41" s="52"/>
-      <c r="C41" s="51">
-        <v>773.15</v>
-      </c>
-      <c r="D41" s="9">
-        <v>0</v>
-      </c>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
+      <c r="A41" s="43"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="52">
-        <v>31.12</v>
-      </c>
-      <c r="B42" s="52"/>
-      <c r="C42" s="51">
-        <v>873.15</v>
-      </c>
-      <c r="D42" s="9">
-        <v>0</v>
-      </c>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="52"/>
-      <c r="B43" s="52"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="52"/>
-      <c r="B44" s="52"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="52"/>
-      <c r="B45" s="52"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="52"/>
-      <c r="B46" s="52"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="43"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="52"/>
-      <c r="B47" s="52"/>
+      <c r="A47" s="43"/>
+      <c r="B47" s="43"/>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="52"/>
-      <c r="B48" s="52"/>
+      <c r="A48" s="43"/>
+      <c r="B48" s="43"/>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="52"/>
-      <c r="B49" s="52"/>
+      <c r="A49" s="43"/>
+      <c r="B49" s="43"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="52"/>
-      <c r="B50" s="52"/>
+      <c r="A50" s="43"/>
+      <c r="B50" s="43"/>
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-    </row>
-    <row r="51" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="42" t="s">
-        <v>47</v>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+    </row>
+    <row r="51" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="38" t="s">
+        <v>25</v>
       </c>
       <c r="B52" s="9"/>
-      <c r="C52" s="31" t="s">
-        <v>125</v>
+      <c r="C52" s="28" t="s">
+        <v>93</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="E52"/>
     </row>
-    <row r="53" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="42" t="s">
-        <v>53</v>
+    <row r="53" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="38" t="s">
+        <v>31</v>
       </c>
       <c r="B53" s="9"/>
-      <c r="C53" s="31" t="s">
-        <v>126</v>
+      <c r="C53" s="28" t="s">
+        <v>94</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="E53"/>
     </row>
-    <row r="54" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="B54" s="20"/>
-      <c r="C54" s="31" t="s">
-        <v>74</v>
+    <row r="54" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B54" s="18"/>
+      <c r="C54" s="28" t="s">
+        <v>46</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="E54"/>
     </row>
-    <row r="55" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="40" t="s">
+    <row r="55" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" s="9"/>
+      <c r="C55" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E55"/>
+    </row>
+    <row r="56" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" s="9"/>
+      <c r="C56" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E56"/>
+    </row>
+    <row r="57" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B57" s="9"/>
+      <c r="C57" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E55"/>
-    </row>
-    <row r="56" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E56"/>
-    </row>
-    <row r="57" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="50" t="s">
-        <v>74</v>
-      </c>
       <c r="D57" s="5" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="E57"/>
-      <c r="F57" s="17"/>
-    </row>
-    <row r="58" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F57" s="15"/>
+    </row>
+    <row r="58" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="8"/>
-      <c r="B58" s="11"/>
       <c r="C58"/>
       <c r="D58"/>
       <c r="E58" s="5"/>
     </row>
-    <row r="59" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B59" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C59" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="D59" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="E59" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="52"/>
-      <c r="B60" s="52"/>
+    <row r="59" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D59" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="43"/>
+      <c r="B60" s="43"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
     </row>
-    <row r="61" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="52"/>
-      <c r="B61" s="52"/>
+    <row r="61" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="43"/>
+      <c r="B61" s="43"/>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
     </row>
-    <row r="62" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="52"/>
-      <c r="B62" s="52"/>
+    <row r="62" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="43"/>
+      <c r="B62" s="43"/>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
     </row>
-    <row r="63" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="52"/>
-      <c r="B63" s="52"/>
+    <row r="63" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="43"/>
+      <c r="B63" s="43"/>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
     </row>
-    <row r="64" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="52"/>
-      <c r="B64" s="52"/>
-      <c r="C64" s="51"/>
+    <row r="64" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="43"/>
+      <c r="B64" s="43"/>
+      <c r="C64" s="42"/>
       <c r="D64" s="9"/>
     </row>
-    <row r="65" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="52"/>
-      <c r="B65" s="52"/>
-      <c r="C65" s="51"/>
+    <row r="65" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="43"/>
+      <c r="B65" s="43"/>
+      <c r="C65" s="42"/>
       <c r="D65" s="9"/>
     </row>
-    <row r="66" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="52"/>
-      <c r="B66" s="52"/>
-      <c r="C66" s="51"/>
+    <row r="66" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="43"/>
+      <c r="B66" s="43"/>
+      <c r="C66" s="42"/>
       <c r="D66" s="9"/>
     </row>
-    <row r="67" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="52"/>
-      <c r="B67" s="52"/>
-      <c r="C67" s="51"/>
+    <row r="67" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="43"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="42"/>
       <c r="D67" s="9"/>
     </row>
-    <row r="68" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="52"/>
-      <c r="B68" s="52"/>
+    <row r="68" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="43"/>
+      <c r="B68" s="43"/>
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
     </row>
-    <row r="69" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="52"/>
-      <c r="B69" s="52"/>
+    <row r="69" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="43"/>
+      <c r="B69" s="43"/>
       <c r="C69" s="9"/>
       <c r="D69" s="9"/>
     </row>
-    <row r="70" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="52"/>
-      <c r="B70" s="52"/>
+    <row r="70" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="43"/>
+      <c r="B70" s="43"/>
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
     </row>
-    <row r="71" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="52"/>
-      <c r="B71" s="52"/>
+    <row r="71" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="43"/>
+      <c r="B71" s="43"/>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
     </row>
-    <row r="72" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="52"/>
-      <c r="B72" s="52"/>
+    <row r="72" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="43"/>
+      <c r="B72" s="43"/>
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
     </row>
-    <row r="73" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="52"/>
-      <c r="B73" s="52"/>
+    <row r="73" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="43"/>
+      <c r="B73" s="43"/>
       <c r="C73" s="9"/>
       <c r="D73" s="9"/>
     </row>
-    <row r="74" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="52"/>
-      <c r="B74" s="52"/>
+    <row r="74" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="43"/>
+      <c r="B74" s="43"/>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
     </row>
-    <row r="75" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="52"/>
-      <c r="B75" s="52"/>
+    <row r="75" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="43"/>
+      <c r="B75" s="43"/>
       <c r="C75" s="9"/>
       <c r="D75" s="9"/>
     </row>
-    <row r="76" spans="1:4" s="61" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="77" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="81" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="82" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="83" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="84" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="85" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="86" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="87" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="88" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="89" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="90" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="91" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="92" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="93" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="94" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="95" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="96" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="97" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="98" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="99" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="100" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="101" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="102" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="103" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="104" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="105" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="106" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="107" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="108" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="109" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="110" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="111" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="112" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="113" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="114" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="115" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="116" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="117" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="118" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="119" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="120" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="121" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="122" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="123" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="124" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="125" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="126" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="127" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="128" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="129" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="130" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="131" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="132" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="81" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="82" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="83" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="84" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="85" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="86" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="87" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="88" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="89" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="90" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="91" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="92" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="93" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="94" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="95" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="96" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="97" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="98" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="99" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="100" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="101" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="102" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="103" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="104" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="105" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="106" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="107" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="108" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="109" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="110" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="111" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="112" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="113" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="114" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="115" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="116" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="117" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="118" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="119" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="120" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="121" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="122" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="123" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="124" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="125" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="126" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="127" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="128" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="129" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="130" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="131" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="132" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B27 B52" xr:uid="{A0BF1BEF-0696-864B-BDBB-F02F002EAA73}">

</xml_diff>